<commit_message>
updoot and pl hw1
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="367">
   <si>
     <t>Programming Languages</t>
   </si>
@@ -41,6 +41,15 @@
     <t>Assignment 1 due Sep 28</t>
   </si>
   <si>
+    <t>ungraded assignment email prof</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>quiz</t>
+  </si>
+  <si>
     <t>Mon</t>
   </si>
   <si>
@@ -62,11 +71,9 @@
     <t>Sun</t>
   </si>
   <si>
-    <t>10-12 wifi installation</t>
-  </si>
-  <si>
-    <t>DS quiz
-DS survey</t>
+    <t>pl hw
+PL notes
+start on flex+bison</t>
   </si>
   <si>
     <t>PL assignment 1 due</t>
@@ -2821,8 +2828,8 @@
   <sheetPr/>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2856,9 +2863,15 @@
       </c>
       <c r="K1" s="59"/>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:6">
       <c r="B2" s="58" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:12">
@@ -2867,7 +2880,9 @@
       <c r="C3" s="58"/>
       <c r="D3" s="58"/>
       <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
+      <c r="F3" s="58" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="58"/>
       <c r="H3" s="58"/>
       <c r="I3" s="58"/>
@@ -2933,36 +2948,42 @@
     </row>
     <row r="8" s="57" customFormat="1" ht="42" customHeight="1" spans="3:9">
       <c r="C8" s="59" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F8" s="59" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G8" s="59" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H8" s="59" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I8" s="59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" ht="100" customHeight="1" spans="2:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" ht="100" customHeight="1" spans="2:9">
       <c r="B9" s="57">
         <v>18</v>
       </c>
-      <c r="D9" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>13</v>
+      <c r="F9" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" ht="100" customHeight="1" spans="2:6">
@@ -2970,12 +2991,12 @@
         <v>25</v>
       </c>
       <c r="F10" s="60" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" ht="100" customHeight="1" spans="1:2">
       <c r="A11" s="57" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" s="57">
         <v>2</v>
@@ -2986,10 +3007,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="58" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" ht="100" customHeight="1" spans="2:2">
@@ -3057,13 +3078,13 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" spans="2:4">
       <c r="B1" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3090,20 +3111,20 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="3:3">
@@ -3166,25 +3187,25 @@
     <row r="2" s="29" customFormat="1" spans="1:13">
       <c r="A2" s="35"/>
       <c r="B2" s="36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -3238,7 +3259,7 @@
       <c r="H6" s="41"/>
       <c r="I6" s="28"/>
       <c r="J6" s="28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
@@ -3255,7 +3276,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="J7" s="28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" s="29" customFormat="1" spans="1:13">
@@ -3271,7 +3292,7 @@
       <c r="H8" s="41"/>
       <c r="I8" s="28"/>
       <c r="J8" s="56" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
@@ -3288,7 +3309,7 @@
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
       <c r="J9" s="28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3303,7 +3324,7 @@
       <c r="G10" s="41"/>
       <c r="H10" s="41"/>
       <c r="J10" s="28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3317,7 +3338,7 @@
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
       <c r="J11" s="28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" s="29" customFormat="1" spans="1:13">
@@ -3333,7 +3354,7 @@
       <c r="H12" s="41"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
@@ -3391,7 +3412,7 @@
       <c r="H16" s="41"/>
       <c r="I16" s="28"/>
       <c r="J16" s="56" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
@@ -3408,7 +3429,7 @@
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
       <c r="J17" s="28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K17" s="28">
         <v>8</v>
@@ -3427,7 +3448,7 @@
       <c r="H18" s="41"/>
       <c r="I18" s="28"/>
       <c r="J18" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K18" s="28">
         <v>3</v>
@@ -3446,7 +3467,7 @@
       <c r="F19" s="33"/>
       <c r="G19" s="33"/>
       <c r="J19" s="28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K19" s="28">
         <v>2</v>
@@ -3465,7 +3486,7 @@
       <c r="H20" s="41"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K20" s="28">
         <v>2</v>
@@ -3479,16 +3500,16 @@
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G21" s="33"/>
       <c r="J21" s="56" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K21" s="28">
         <v>4</v>
@@ -3507,7 +3528,7 @@
       <c r="H22" s="41"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K22" s="28">
         <v>5</v>
@@ -3535,7 +3556,7 @@
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
@@ -3556,7 +3577,7 @@
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E25" s="44"/>
       <c r="F25" s="33"/>
@@ -3598,7 +3619,7 @@
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
       <c r="E28" s="45" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
@@ -3709,25 +3730,25 @@
     <row r="41" spans="1:8">
       <c r="A41" s="35"/>
       <c r="B41" s="36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F41" s="36" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G41" s="36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H41" s="37" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4103,172 +4124,172 @@
   <sheetData>
     <row r="3" s="16" customFormat="1" spans="2:8">
       <c r="B3" s="20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="F3" s="21"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" s="17" customFormat="1" spans="2:9">
       <c r="B4" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" s="8" customFormat="1" spans="2:9">
       <c r="B8" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" s="8" customFormat="1" spans="2:8">
       <c r="B9" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" s="8" customFormat="1" spans="3:8">
       <c r="C10" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" s="8" customFormat="1" spans="3:7">
       <c r="C11" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G11" s="19"/>
     </row>
     <row r="12" s="8" customFormat="1" spans="3:7">
       <c r="C12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G12" s="19"/>
     </row>
     <row r="13" s="8" customFormat="1" spans="3:7">
       <c r="C13" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G13" s="19"/>
     </row>
     <row r="14" s="8" customFormat="1" spans="3:7">
       <c r="C14" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G14" s="19"/>
     </row>
@@ -4278,7 +4299,7 @@
     <row r="16" s="8" customFormat="1" spans="7:13">
       <c r="G16" s="19"/>
       <c r="H16" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M16" s="8">
         <v>59</v>
@@ -4287,7 +4308,7 @@
     <row r="17" s="8" customFormat="1" spans="7:13">
       <c r="G17" s="19"/>
       <c r="H17" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M17" s="8">
         <v>58</v>
@@ -4296,7 +4317,7 @@
     <row r="18" s="8" customFormat="1" spans="7:13">
       <c r="G18" s="19"/>
       <c r="H18" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="M18" s="8">
         <v>57</v>
@@ -4305,7 +4326,7 @@
     <row r="19" s="8" customFormat="1" spans="7:13">
       <c r="G19" s="19"/>
       <c r="H19" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M19" s="8">
         <v>56</v>
@@ -4314,7 +4335,7 @@
     <row r="20" s="8" customFormat="1" spans="7:13">
       <c r="G20" s="19"/>
       <c r="H20" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M20" s="8">
         <v>55</v>
@@ -4323,7 +4344,7 @@
     <row r="21" s="8" customFormat="1" spans="7:13">
       <c r="G21" s="19"/>
       <c r="H21" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="M21" s="8">
         <v>54</v>
@@ -4332,19 +4353,19 @@
     <row r="22" s="8" customFormat="1" spans="7:8">
       <c r="G22" s="19"/>
       <c r="H22" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" s="8" customFormat="1" spans="7:8">
       <c r="G23" s="19"/>
       <c r="H23" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" s="8" customFormat="1" spans="7:8">
       <c r="G24" s="19"/>
       <c r="H24" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" s="8" customFormat="1" spans="7:7">
@@ -4355,121 +4376,121 @@
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" s="18" customFormat="1" ht="38.25" spans="2:9">
       <c r="B34" s="24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G34" s="26"/>
       <c r="I34" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" s="18" customFormat="1" ht="38.25" spans="2:9">
       <c r="B35" s="25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G35" s="26"/>
       <c r="I35" s="25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" s="18" customFormat="1" ht="51" spans="2:9">
       <c r="B36" s="25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" s="18" customFormat="1" ht="51" spans="2:8">
       <c r="B37" s="25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H37" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" s="18" customFormat="1" ht="38.25" spans="2:8">
       <c r="B38" s="25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
       <c r="E38" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G38" s="26"/>
       <c r="H38" s="25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" s="18" customFormat="1" ht="38.25" spans="2:7">
       <c r="B39" s="25" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -4477,7 +4498,7 @@
     </row>
     <row r="40" s="18" customFormat="1" ht="38.25" spans="2:7">
       <c r="B40" s="25" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
@@ -4518,284 +4539,284 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="3:8">
       <c r="C3" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="11"/>
       <c r="C4" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="12"/>
       <c r="C5" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="13"/>
       <c r="C6" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="14"/>
       <c r="C7" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="15"/>
       <c r="C8" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="3:7">
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="3:7">
       <c r="C10" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="3:5">
       <c r="C19" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="3:5">
       <c r="C20" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="3:5">
       <c r="C21" s="8" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="3:5">
       <c r="C22" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="3:5">
       <c r="C23" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" s="8" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" s="8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="3:3">
       <c r="C28" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="3:3">
       <c r="C29" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" s="8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" s="8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" s="7" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" s="8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" s="8" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" s="8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="3:3">
       <c r="C41" s="8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="3:3">
       <c r="C42" s="8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4820,174 +4841,174 @@
   <sheetData>
     <row r="1" s="7" customFormat="1" ht="15" customHeight="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="4:4">
       <c r="D12" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="4:4">
       <c r="D13" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="4:4">
       <c r="D14" s="8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="4:4">
       <c r="D15" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:1">
       <c r="A16" s="8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:1">
       <c r="A17" s="8" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -5012,80 +5033,80 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -5116,388 +5137,388 @@
   <sheetData>
     <row r="2" s="2" customFormat="1" spans="2:6">
       <c r="B2" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5524,46 +5545,46 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="F4" s="1">
         <v>14999</v>
@@ -5571,26 +5592,26 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5618,37 +5639,37 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" ht="80" customHeight="1" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" ht="80" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>